<commit_message>
Refactor document templates and placeholder logic
Removed old document files and moved templates to 'charm-docs-template' directory. Added and updated scripts for placeholder replacement in Word documents. Improved placeholder handling and document generation logic in 'generate_charm_docs.py'. Updated Excel data and streamlined template usage for output generation.
</commit_message>
<xml_diff>
--- a/charm_data.xlsx
+++ b/charm_data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seema\Desktop\AI\charm_doc_generator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5747DA78-0D2C-41EE-8F72-EFB60C9B24F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Program Name</t>
   </si>
@@ -58,41 +64,65 @@
     <t>Test Result Reviewed By</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Screenshot Path</t>
   </si>
   <si>
-    <t>ZGR_INDAS_CFS_RS_CRS_FINAL</t>
-  </si>
-  <si>
-    <t>Harshit Dixit</t>
-  </si>
-  <si>
-    <t>ZGR_INDAS_CONSOLIDATED_FINANCIALS</t>
-  </si>
-  <si>
-    <t>Changes in existing report as per user requirement.</t>
-  </si>
-  <si>
-    <t>New report according to user specification</t>
-  </si>
-  <si>
-    <t>Jyosyula Siva Amrutha</t>
-  </si>
-  <si>
-    <t>Swagata Roy</t>
-  </si>
-  <si>
-    <t>Indraneel Mazumder</t>
-  </si>
-  <si>
     <t>C:/Users/seema/Pictures/Screenshots/Screenshots(2).png</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +134,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,13 +191,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +243,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -233,6 +277,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -267,9 +312,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,14 +488,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,55 +543,62 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2">
-        <v>2025007382</v>
-      </c>
-      <c r="D2">
-        <v>2025007376</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code for robust handling
</commit_message>
<xml_diff>
--- a/charm_data.xlsx
+++ b/charm_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seema\Desktop\AI\charm_doc_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI Learning\charm-doc-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5747DA78-0D2C-41EE-8F72-EFB60C9B24F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D3024D-290F-4430-8D7B-D89CC8DEF7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Program Name</t>
   </si>
@@ -70,52 +70,46 @@
     <t>Screenshot Path</t>
   </si>
   <si>
-    <t>C:/Users/seema/Pictures/Screenshots/Screenshots(2).png</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>A13</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t>A16</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Harshit</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>make report</t>
+  </si>
+  <si>
+    <t>make afo report</t>
+  </si>
+  <si>
+    <t>HarshitPlan</t>
+  </si>
+  <si>
+    <t>HarshitPlanReview</t>
+  </si>
+  <si>
+    <t>HarshitTest</t>
+  </si>
+  <si>
+    <t>HarshitTestReview</t>
+  </si>
+  <si>
+    <t>TRP</t>
+  </si>
+  <si>
+    <t>TRR</t>
+  </si>
+  <si>
+    <t>18.07.2025</t>
+  </si>
+  <si>
+    <t>"D:\OneDrive - Tata Steel Limited\Pictures\Screenshots\Screenshot (255).png"</t>
   </si>
 </sst>
 </file>
@@ -180,10 +174,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,109 +490,115 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" customWidth="1"/>
+    <col min="16" max="16" width="9.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <v>456</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>